<commit_message>
dev için dinamik pin ekleme
dev için excelden gelen pin değerleri dinamik  bir şekilde eklendi. Blokların saysız  bunlar göre oluştu.
</commit_message>
<xml_diff>
--- a/ExcelToJSON/ornek.xlsx
+++ b/ExcelToJSON/ornek.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFBF7271-70A0-412C-9EA2-367C91A25C5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E25C9842-B7EB-4B65-887F-FC10EE5D2828}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3375" yWindow="3375" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="54">
   <si>
     <t>Signal</t>
   </si>
@@ -193,6 +193,9 @@
   </si>
   <si>
     <t>282108-1</t>
+  </si>
+  <si>
+    <t>282107-1</t>
   </si>
 </sst>
 </file>
@@ -401,6 +404,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -412,12 +421,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -440,23 +443,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>375767</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>131884</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>630613</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>74265</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>572580</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>152924</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="4" name="Resim 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7EC833A6-E6ED-4A23-8C0E-90AF42CC5A81}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C53317EF-58AC-9D8C-B2E9-1D9D3D0CD3C1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -472,8 +475,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3965959" y="2227384"/>
-          <a:ext cx="7742962" cy="3752381"/>
+          <a:off x="13668375" y="2305050"/>
+          <a:ext cx="7735380" cy="3753374"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -751,10 +754,10 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:V7"/>
+  <dimension ref="A1:V8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3:T7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -791,28 +794,28 @@
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="4"/>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="13"/>
-      <c r="H1" s="14" t="s">
+      <c r="G1" s="15"/>
+      <c r="H1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="15" t="s">
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
       <c r="V1" s="5"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
@@ -887,7 +890,7 @@
       <c r="A3" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="12" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="9" t="s">
@@ -908,7 +911,7 @@
       <c r="H3" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="I3" s="12" t="s">
         <v>25</v>
       </c>
       <c r="J3" s="9" t="s">
@@ -920,7 +923,7 @@
       <c r="L3" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="M3" s="17" t="s">
+      <c r="M3" s="13" t="s">
         <v>52</v>
       </c>
       <c r="N3" s="11">
@@ -941,7 +944,7 @@
       <c r="S3" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="T3" s="17" t="s">
+      <c r="T3" s="13" t="s">
         <v>52</v>
       </c>
       <c r="U3" s="9">
@@ -955,7 +958,7 @@
       <c r="A4" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="12" t="s">
         <v>34</v>
       </c>
       <c r="C4" s="9" t="s">
@@ -976,7 +979,7 @@
       <c r="H4" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="16" t="s">
+      <c r="I4" s="12" t="s">
         <v>36</v>
       </c>
       <c r="J4" s="9" t="s">
@@ -988,8 +991,8 @@
       <c r="L4" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="M4" s="17" t="s">
-        <v>52</v>
+      <c r="M4" s="13" t="s">
+        <v>53</v>
       </c>
       <c r="N4" s="11">
         <v>2</v>
@@ -1009,8 +1012,8 @@
       <c r="S4" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="T4" s="17" t="s">
-        <v>52</v>
+      <c r="T4" s="13" t="s">
+        <v>53</v>
       </c>
       <c r="U4" s="9">
         <v>2</v>
@@ -1023,7 +1026,7 @@
       <c r="A5" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="12" t="s">
         <v>38</v>
       </c>
       <c r="C5" s="9" t="s">
@@ -1044,7 +1047,7 @@
       <c r="H5" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="16" t="s">
+      <c r="I5" s="12" t="s">
         <v>43</v>
       </c>
       <c r="J5" s="9" t="s">
@@ -1056,7 +1059,7 @@
       <c r="L5" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="M5" s="17" t="s">
+      <c r="M5" s="13" t="s">
         <v>52</v>
       </c>
       <c r="N5" s="11" t="s">
@@ -1077,7 +1080,7 @@
       <c r="S5" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="T5" s="17" t="s">
+      <c r="T5" s="13" t="s">
         <v>52</v>
       </c>
       <c r="U5" s="9" t="s">
@@ -1091,7 +1094,7 @@
       <c r="A6" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="12" t="s">
         <v>45</v>
       </c>
       <c r="C6" s="9" t="s">
@@ -1112,7 +1115,7 @@
       <c r="H6" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="I6" s="16" t="s">
+      <c r="I6" s="12" t="s">
         <v>46</v>
       </c>
       <c r="J6" s="9" t="s">
@@ -1124,7 +1127,7 @@
       <c r="L6" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="M6" s="17" t="s">
+      <c r="M6" s="13" t="s">
         <v>52</v>
       </c>
       <c r="N6" s="11" t="s">
@@ -1145,7 +1148,7 @@
       <c r="S6" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="T6" s="17" t="s">
+      <c r="T6" s="13" t="s">
         <v>52</v>
       </c>
       <c r="U6" s="9" t="s">
@@ -1159,7 +1162,7 @@
       <c r="A7" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="12" t="s">
         <v>49</v>
       </c>
       <c r="C7" s="9" t="s">
@@ -1180,7 +1183,7 @@
       <c r="H7" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="I7" s="16" t="s">
+      <c r="I7" s="12" t="s">
         <v>50</v>
       </c>
       <c r="J7" s="9" t="s">
@@ -1192,7 +1195,7 @@
       <c r="L7" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="M7" s="17" t="s">
+      <c r="M7" s="13" t="s">
         <v>52</v>
       </c>
       <c r="N7" s="11" t="s">
@@ -1213,13 +1216,81 @@
       <c r="S7" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="T7" s="17" t="s">
+      <c r="T7" s="13" t="s">
         <v>52</v>
       </c>
       <c r="U7" s="9" t="s">
         <v>51</v>
       </c>
       <c r="V7" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="9">
+        <v>5</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="K8" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="L8" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M8" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="N8" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="O8" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="P8" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q8" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="R8" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="S8" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="T8" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="U8" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="V8" s="9" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1232,19 +1303,19 @@
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="C3:C7" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="C3:C8" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"28VDC POWER,RETURN,1553 MUX BUS,ANALOG,ARINC 429,CHASSIS GROUND,ETHERNET,RS485,DISCRETE 28VDC OPEN,DISCRETE GND OPEN,VIDEO,N/A"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="D3:E7" xr:uid="{00000000-0002-0000-0000-000006000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="D3:E8" xr:uid="{00000000-0002-0000-0000-000006000000}">
       <formula1>"A Route - Power,C Route - low level sıgnal,D Route - Dıgıtal Sıgnals,S Route - Sensıtıve,N/A"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="B3:B7 O3:Q7 H3:J7" xr:uid="{00000000-0002-0000-0000-000007000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="B3:B8 O3:Q8 H3:J8" xr:uid="{00000000-0002-0000-0000-000007000000}">
       <formula1>"ATA21,ATA23,ATA24,ATA26,ATA27,ATA28,ATA29,ATA30,ATA31,ATA32,ATA33,ATA34,ATA35,ATA46,ATA51,ATA52,ATA60-80,ATA95,ATA45,N/A"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="G3:G7" xr:uid="{00000000-0002-0000-0000-000008000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="G3:G8" xr:uid="{00000000-0002-0000-0000-000008000000}">
       <formula1>"0,2,4,6,8,10,12,14,16,18,20,22,24,26,28,N/A"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="F3:F7" xr:uid="{00000000-0002-0000-0000-000009000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="F3:F8" xr:uid="{00000000-0002-0000-0000-000009000000}">
       <formula1>"SıngleWire,SıngleShielded,ShıeldTwısted,Twısted,Triax,Coaxial,N/A"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>